<commit_message>
fix bug in specific stat and socket stat
</commit_message>
<xml_diff>
--- a/tasks/task_table_cold.xlsx
+++ b/tasks/task_table_cold.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="51">
   <si>
     <t>SEGMENT</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -218,6 +218,10 @@
   </si>
   <si>
     <t>c40_minus_c100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>head</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -692,11 +696,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1762,7 +1766,7 @@
     </row>
     <row r="44" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>16</v>
@@ -1788,16 +1792,16 @@
         <v>7</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E45" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J45" s="5">
         <v>0</v>
@@ -1820,7 +1824,7 @@
         <v>17</v>
       </c>
       <c r="E46" s="5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J46" s="5">
         <v>0</v>
@@ -1843,12 +1847,35 @@
         <v>17</v>
       </c>
       <c r="E47" s="5">
+        <v>18</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="5">
         <v>20</v>
       </c>
-      <c r="J47" s="5">
-        <v>0</v>
-      </c>
-      <c r="K47" s="5" t="s">
+      <c r="J48" s="5">
+        <v>0</v>
+      </c>
+      <c r="K48" s="5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>